<commit_message>
Nav Screen disappeared on Home Page
</commit_message>
<xml_diff>
--- a/Notes/pricing.xlsx
+++ b/Notes/pricing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Sizes</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Winter Snoods</t>
   </si>
   <si>
-    <t>Snoods</t>
-  </si>
-  <si>
     <t>Pee Wraps</t>
   </si>
   <si>
@@ -91,6 +88,24 @@
   </si>
   <si>
     <t>Warming Coats*</t>
+  </si>
+  <si>
+    <t>Snoods/Bibs</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Diapers</t>
+  </si>
+  <si>
+    <t>Belly Bands</t>
+  </si>
+  <si>
+    <t>Bibs</t>
+  </si>
+  <si>
+    <t>Bellybands</t>
   </si>
 </sst>
 </file>
@@ -134,9 +149,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -440,488 +458,527 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="2" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="11" width="19.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15" customWidth="1"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C2">
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="E3">
         <v>80</v>
       </c>
-      <c r="C3">
+      <c r="F3">
         <v>60</v>
       </c>
-      <c r="D3">
-        <f>+C3</f>
+      <c r="G3">
+        <f>+F3</f>
         <v>60</v>
       </c>
-      <c r="E3">
-        <f>+B3</f>
-        <v>80</v>
-      </c>
-      <c r="F3">
-        <v>120</v>
-      </c>
-      <c r="G3">
-        <f>+F3+15</f>
-        <v>135</v>
-      </c>
       <c r="H3">
-        <v>25</v>
-      </c>
-      <c r="I3">
-        <f>+H3+15</f>
-        <v>40</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3">
         <f>+E3</f>
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>120</v>
+      </c>
+      <c r="J3">
+        <f>+I3+15</f>
+        <v>135</v>
+      </c>
+      <c r="K3">
+        <v>25</v>
+      </c>
+      <c r="L3">
+        <f>+K3+15</f>
+        <v>40</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3">
+        <f>+H3</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="E4">
         <v>80</v>
       </c>
-      <c r="C4">
+      <c r="F4">
         <v>60</v>
       </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D11" si="0">+C4</f>
+      <c r="G4">
+        <f t="shared" ref="G4:G11" si="0">+F4</f>
         <v>60</v>
       </c>
-      <c r="E4">
-        <f t="shared" ref="E4:E11" si="1">+B4</f>
+      <c r="H4">
+        <f t="shared" ref="H4:H11" si="1">+E4</f>
         <v>80</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>120</v>
       </c>
-      <c r="G4">
-        <f t="shared" ref="G4:G11" si="2">+F4+15</f>
+      <c r="J4">
+        <f t="shared" ref="J4:J11" si="2">+I4+15</f>
         <v>135</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>25</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4:I11" si="3">+H4+15</f>
+      <c r="L4">
+        <f t="shared" ref="L4:L11" si="3">+K4+15</f>
         <v>40</v>
       </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M11" si="4">+E4</f>
+      <c r="M4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P11" si="4">+H4</f>
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="E5">
         <v>80</v>
       </c>
-      <c r="C5">
+      <c r="F5">
         <v>60</v>
       </c>
-      <c r="D5">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>120</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <f t="shared" si="2"/>
         <v>135</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>25</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5">
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="4"/>
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="E6">
         <v>95</v>
       </c>
-      <c r="C6">
+      <c r="F6">
         <v>75</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="F6">
-        <f>+F5+15</f>
+      <c r="I6">
+        <f>+I5+15</f>
         <v>135</v>
       </c>
-      <c r="G6">
+      <c r="J6">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>25</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6">
+      <c r="M6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6">
         <v>70</v>
       </c>
-      <c r="L6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6">
+      <c r="O6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="4"/>
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="E7">
         <v>110</v>
       </c>
-      <c r="C7">
+      <c r="F7">
         <v>90</v>
       </c>
-      <c r="D7">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="E7">
+      <c r="H7">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="F7">
-        <f t="shared" ref="F7:F11" si="5">+F6+15</f>
+      <c r="I7">
+        <f t="shared" ref="I7:I11" si="5">+I6+15</f>
         <v>150</v>
       </c>
-      <c r="G7">
+      <c r="J7">
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>35</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="J7">
+      <c r="M7">
         <v>70</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>70</v>
       </c>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7">
+      <c r="O7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="4"/>
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="E8">
         <v>125</v>
       </c>
-      <c r="C8">
+      <c r="F8">
         <v>105</v>
       </c>
-      <c r="D8">
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="E8">
+      <c r="H8">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="F8">
+      <c r="I8">
         <f t="shared" si="5"/>
         <v>165</v>
       </c>
-      <c r="G8">
+      <c r="J8">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>35</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="J8">
+      <c r="M8">
         <v>70</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>70</v>
       </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8">
+      <c r="O8" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="4"/>
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="E9">
         <v>140</v>
       </c>
-      <c r="C9">
+      <c r="F9">
         <v>120</v>
       </c>
-      <c r="D9">
+      <c r="G9">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="E9">
+      <c r="H9">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <f t="shared" si="5"/>
         <v>180</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <f t="shared" si="2"/>
         <v>195</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>35</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="J9">
+      <c r="M9">
         <v>70</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>70</v>
       </c>
-      <c r="L9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9">
+      <c r="O9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="4"/>
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="E10">
         <v>155</v>
       </c>
-      <c r="C10">
+      <c r="F10">
         <v>135</v>
       </c>
-      <c r="D10">
+      <c r="G10">
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
-      <c r="E10">
+      <c r="H10">
         <f t="shared" si="1"/>
         <v>155</v>
       </c>
-      <c r="F10">
+      <c r="I10">
         <f t="shared" si="5"/>
         <v>195</v>
       </c>
-      <c r="G10">
+      <c r="J10">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="H10">
+      <c r="K10">
         <v>35</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="J10">
+      <c r="M10">
         <v>70</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>70</v>
       </c>
-      <c r="L10" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10">
+      <c r="O10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="4"/>
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="E11">
         <v>170</v>
       </c>
-      <c r="C11">
+      <c r="F11">
         <v>150</v>
       </c>
-      <c r="D11">
+      <c r="G11">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="E11">
+      <c r="H11">
         <f t="shared" si="1"/>
         <v>170</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <f t="shared" si="5"/>
         <v>210</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <f t="shared" si="2"/>
         <v>225</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>35</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="J11">
+      <c r="M11">
         <v>70</v>
       </c>
-      <c r="K11">
+      <c r="N11">
         <v>70</v>
       </c>
-      <c r="L11" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11">
+      <c r="O11" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="4"/>
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>